<commit_message>
Bosses come out of a multiple of 10
</commit_message>
<xml_diff>
--- a/Data/SpawnData.xlsx
+++ b/Data/SpawnData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\BroGame\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF4494F-5C79-4C8A-8B4F-7311FBCD89A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F0CBCD-51E3-40B2-8427-899FE01A01BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6F927B04-BACA-48DB-BEF1-E78F9F00866E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{85F11096-AC3F-4D9D-B598-BE09DDB71694}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,37 +31,58 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>Quantity</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ClassName</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>("/Game/Character/Monster/BMonster_BP.BMonster_BP_C", "/Game/Character/Monster/BMonster_BP.BMonster_BP_C", "/Game/Character/Monster/BMonster_BP2.BMonster_BP2_C")</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(3, 2, 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>("/Game/Character/Monster/BMonster_BP2.BMonster_BP2_C", "/Game/Character/Monster/BMonster_BP.BMonster_BP_C")</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(3, 1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>("/Game/Character/Monster/BMonster_BP2.BMonster_BP2_C")</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
+  <si>
+    <t>Num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Damage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaxHP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Speed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Size</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Wave</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MonsterClassPath</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>("/Game/Character/Monster/WhiteMinion/BWhiteMinion_BP.BWhiteMinion_BP_C")</t>
+  </si>
+  <si>
+    <t>("/Game/Character/Monster/SuperMinion/BSuperMinion_BP.BSuperMinion_BP_C", "/Game/Character/Monster/SuperMinion/BSuperMinion_BP.BSuperMinion_BP_C", "/Game/Character/Monster/WhiteMinion/BWhiteMinion_BP.BWhiteMinion_BP_C")</t>
+  </si>
+  <si>
+    <t>(1, 2, 3)</t>
+  </si>
+  <si>
+    <t>(50, 20, 50)</t>
+  </si>
+  <si>
+    <t>(100, 200, 300)</t>
+  </si>
+  <si>
+    <t>(200, 300, 400)</t>
+  </si>
+  <si>
+    <t>(1, 1, 1)</t>
+  </si>
+  <si>
+    <t>DropMoney</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -70,7 +91,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="182" formatCode="0_);\(0\)"/>
+    <numFmt numFmtId="176" formatCode="0_);\(0\)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -116,10 +137,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -434,99 +455,174 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B85D6A83-F3B0-4494-9D7B-406D6909DB30}">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD86482F-868F-4E0C-B33D-E3D15ED44C48}">
+  <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="50.1" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="99.125" customWidth="1"/>
-    <col min="4" max="4" width="62.125" customWidth="1"/>
-    <col min="6" max="6" width="65.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="72" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2">
+        <v>-9</v>
+      </c>
+      <c r="D2" s="2">
+        <v>-50</v>
+      </c>
+      <c r="E2" s="2">
+        <v>-10</v>
+      </c>
+      <c r="F2" s="2">
+        <v>-200</v>
+      </c>
+      <c r="G2" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H2" s="2">
+        <v>-10</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2">
+        <v>-20</v>
+      </c>
+      <c r="D3" s="2">
+        <v>-10</v>
+      </c>
+      <c r="E3" s="2">
+        <v>-50</v>
+      </c>
+      <c r="F3" s="2">
+        <v>-400</v>
+      </c>
+      <c r="G3" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>-100</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="2">
-        <v>-3</v>
-      </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" ht="50.1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>